<commit_message>
Actualización del excel de seguimiento de tareas "Carolina Arce.xlsx" y "Carolina Arce.xls"
</commit_message>
<xml_diff>
--- a/Requerimientos/CUS 46 - Facturar Pago de Tarifa Aeroportuario por Pasaje de Aerolínea/Carolina Arce.xlsx
+++ b/Requerimientos/CUS 46 - Facturar Pago de Tarifa Aeroportuario por Pasaje de Aerolínea/Carolina Arce.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505"/>
@@ -11,10 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -93,8 +90,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,9 +248,6 @@
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -294,30 +288,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,9 +304,33 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,28 +347,15 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-PE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="es-ES"/>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -388,7 +372,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -408,52 +392,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="96470144"/>
-        <c:axId val="96471680"/>
+        <c:axId val="64980096"/>
+        <c:axId val="64981632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96470144"/>
+        <c:axId val="64980096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96471680"/>
+        <c:crossAx val="64981632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96471680"/>
+        <c:axId val="64981632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96470144"/>
+        <c:crossAx val="64980096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -461,15 +429,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -510,19 +476,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Hoja1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -600,7 +553,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -635,7 +587,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -811,304 +762,298 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="5">
+      <c r="B2" s="34"/>
+      <c r="C2" s="4">
         <v>15</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="12" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+    <row r="6" spans="1:9">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="18">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="17">
         <v>3</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="18">
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="17">
         <v>4</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="18">
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="17">
         <v>3</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="18">
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="17">
         <v>2</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75">
+      <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="18">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="17">
         <v>3</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="37"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="I10" s="21"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="18">
         <f>SUM(G6:G10)</f>
         <v>15</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="7">
+      <c r="B18" s="28"/>
+      <c r="C18" s="6">
         <f>SUM(C19:C23)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="8">
+      <c r="B24" s="26"/>
+      <c r="C24" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1117,6 +1062,12 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1125,24 +1076,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>